<commit_message>
Ausgabe einer Pause, auch wenn diese nicht stattfinden kann / Klimatisierung während Pause / Verhindern, dass Bus mehrmals an gleicher Bushaltestelle hält
</commit_message>
<xml_diff>
--- a/Inputdateien/Input.xlsx
+++ b/Inputdateien/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\PycharmProjects\Bachelorarbeit_Git\Inputdateien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1567D4-D0C9-4505-B7A0-585C3DF11A25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D701843-2086-437F-A738-9E22B78336D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0BB4CFC-4877-4FD6-BF56-167E70887CDC}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,7 +422,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
@@ -442,18 +442,18 @@
         <v>0</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
-        <v>0.7</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>50</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -464,10 +464,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
-        <v>2.5628000000000002</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -476,18 +476,18 @@
         <v>0</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -498,13 +498,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>5.0999999999999996</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -515,10 +515,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
-        <v>7.3</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="B8" s="2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -531,55 +531,32 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>30</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>9.1</v>
-      </c>
-      <c r="B10" s="2">
-        <v>50</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="B11" s="2">
-        <v>50</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>